<commit_message>
All Spec: Integrated- Working & updated RegisterSpec
</commit_message>
<xml_diff>
--- a/resources/imports/loginTestData.xlsx
+++ b/resources/imports/loginTestData.xlsx
@@ -58,7 +58,7 @@
       <table:table table:name="Register" table:style-name="ta1" table:print="false">
         <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co3" table:number-columns-repeated="3" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co3" table:number-columns-repeated="5" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string">
             <text:p>uname </text:p>
@@ -73,7 +73,13 @@
             <text:p>phone</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string">
-            <text:p>password </text:p>
+            <text:p>pswd </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>business</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>country</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro2">
@@ -92,6 +98,12 @@
           <table:table-cell office:value-type="string">
             <text:p>Atest@123</text:p>
           </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>Hotel</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>Japan</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string">
@@ -109,6 +121,12 @@
           <table:table-cell office:value-type="string">
             <text:p>Btest@123</text:p>
           </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>Flowers</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>Singapore</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string">
@@ -125,6 +143,12 @@
           </table:table-cell>
           <table:table-cell office:value-type="string">
             <text:p>Ctest@123</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>Spa</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string">
+            <text:p>Singapore</text:p>
           </table:table-cell>
         </table:table-row>
       </table:table>
@@ -204,11 +228,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.2">
   <office:meta>
     <meta:creation-date>2019-10-13T17:50:48.01</meta:creation-date>
-    <dc:date>2019-10-14T08:28:56.33</dc:date>
-    <meta:editing-duration>PT11H9M9S</meta:editing-duration>
-    <meta:editing-cycles>7</meta:editing-cycles>
+    <dc:date>2019-11-07T11:40:54.25</dc:date>
+    <meta:editing-duration>PT11H10M54S</meta:editing-duration>
+    <meta:editing-cycles>8</meta:editing-cycles>
     <meta:generator>OpenOffice/4.1.3$Win32 OpenOffice.org_project/413m1$Build-9783</meta:generator>
-    <meta:document-statistic meta:table-count="3" meta:cell-count="35" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="3" meta:cell-count="43" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -219,15 +243,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">13434</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">17950</config:config-item>
       <config:config-item config:name="VisibleAreaHeight" config:type="int">1883</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Register">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">10</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">6</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -437,9 +461,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2019-10-14">10/14/2019</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2019-11-07">11/07/2019</text:date>
             , 
-            <text:time>08:28:56</text:time>
+            <text:time>11:40:54</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>